<commit_message>
pro b admin lock
</commit_message>
<xml_diff>
--- a/stu data.xlsx
+++ b/stu data.xlsx
@@ -208,7 +208,7 @@
     <t xml:space="preserve">dknaix.github@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">admin</t>
+    <t xml:space="preserve">admin_p</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
admin_b also ready testing now
</commit_message>
<xml_diff>
--- a/stu data.xlsx
+++ b/stu data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
   <si>
     <t xml:space="preserve">NAME </t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">admin_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyurramanini@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin_b</t>
   </si>
 </sst>
 </file>
@@ -444,7 +453,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -997,6 +1006,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="6" t="n">
+        <v>1234567890</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
     </row>
@@ -1067,6 +1096,9 @@
       <c r="A57" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" display="keyurramanini@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
basic msg complete test
</commit_message>
<xml_diff>
--- a/stu data.xlsx
+++ b/stu data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t xml:space="preserve">NAME </t>
   </si>
@@ -208,16 +208,13 @@
     <t xml:space="preserve">dknaix.github@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">admin_p</t>
+    <t xml:space="preserve">admin_b</t>
   </si>
   <si>
     <t xml:space="preserve">keyur</t>
   </si>
   <si>
     <t xml:space="preserve">keyurramanini@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin_b</t>
   </si>
 </sst>
 </file>
@@ -453,7 +450,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,7 +1014,7 @@
         <v>1234567890</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
new 5th api for pro admin
</commit_message>
<xml_diff>
--- a/stu data.xlsx
+++ b/stu data.xlsx
@@ -450,7 +450,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -974,7 +974,7 @@
         <v>1234567890</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
admin page post testing
</commit_message>
<xml_diff>
--- a/stu data.xlsx
+++ b/stu data.xlsx
@@ -208,7 +208,7 @@
     <t xml:space="preserve">dknaix.github@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">admin_b</t>
+    <t xml:space="preserve">elite</t>
   </si>
   <si>
     <t xml:space="preserve">keyur</t>
@@ -228,7 +228,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -265,12 +265,6 @@
       <name val="Roboto"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -342,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,10 +367,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -462,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1006,7 +996,7 @@
       <c r="C27" s="6" t="n">
         <v>1234567890</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="0" t="n">
@@ -1026,7 +1016,7 @@
       <c r="C28" s="6" t="n">
         <v>1234567890</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="0" t="n">

</xml_diff>